<commit_message>
re-added in BLEU and GLEU score calculations
</commit_message>
<xml_diff>
--- a/metric.xlsx
+++ b/metric.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Comments</t>
   </si>
@@ -33,6 +33,45 @@
   </si>
   <si>
     <t>Model's replies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> different than what i expected on the outset but i still ended up having a good time with it eos</t>
+  </si>
+  <si>
+    <t>Decoded sequence: sos i the the the the the the</t>
+  </si>
+  <si>
+    <t>Input sequence: sos spring 2015 plastic memories danmachi kekkai sensen only one of those i liked eos</t>
+  </si>
+  <si>
+    <t>Decoded sequence: sos the the the the the the the the the the the the</t>
+  </si>
+  <si>
+    <t>Input sequence: sos to all the saber lovers out there enjoy https imgurcomakdrqu some content is nsfw eos</t>
+  </si>
+  <si>
+    <t>Input sequence: names are and where to start there s lots of good anime out there today some long some short eos</t>
+  </si>
+  <si>
+    <t>Decoded sequence: sos the the the the the the the this</t>
+  </si>
+  <si>
+    <t>Input sequence: sos first and last episodes of plastic memories eos</t>
+  </si>
+  <si>
+    <t>Input sequence: sos winter 2015 and i watched pretty much everything but my favorites were death parade parasyte and yuri kuma eos</t>
+  </si>
+  <si>
+    <t>Input sequence: 20140302110443 and basketball lesbians http i1294photobucketcomalbumsb619isonnazzoanimelarge zpssf3c0razgif also the only one who can kill me is me https smediacacheak0pinimgcom236xdac909dac90980a052e3bde464b4cad968e011jpg eos</t>
+  </si>
+  <si>
+    <t>Input sequence: sos i think you d enjoy psychopass http myanimelistnetanime13601psychopass eos</t>
+  </si>
+  <si>
+    <t>Input sequence: for some reason bears all over the world rose up and attacked humanity yuri kuma was a fun show eos</t>
+  </si>
+  <si>
+    <t>Input sequence: be immersed in the story sadly it s only two episodes and the novel s translation are barely breathing eos</t>
   </si>
 </sst>
 </file>
@@ -350,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A2:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,6 +413,106 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>